<commit_message>
fix hyperlink to file
</commit_message>
<xml_diff>
--- a/testdata/Links.xlsx
+++ b/testdata/Links.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel Howind\IdeaProjects\meja\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D58AA1-8770-405B-AD53-218A9DA9EED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700C8C91-05B8-43F5-9960-8083A9C256CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30300" windowHeight="16540" xr2:uid="{2CD721D7-B6E9-4552-8F83-8DA45E0A885F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Links" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>